<commit_message>
Cargados OUTPUTS versión 1.3
</commit_message>
<xml_diff>
--- a/Project Outputs for Frost5000Beta/BOM Archive/BOM_Frost5000Beta.xlsx
+++ b/Project Outputs for Frost5000Beta/BOM Archive/BOM_Frost5000Beta.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="227">
   <si>
     <t>Component List / BOM Archive</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Version:</t>
   </si>
   <si>
-    <t>Beta 1.0</t>
+    <t>Beta 1.3</t>
   </si>
   <si>
     <t>Website:</t>
@@ -425,10 +425,7 @@
     <t>Resistor SMD</t>
   </si>
   <si>
-    <t>40, 47</t>
-  </si>
-  <si>
-    <t>Ra2, Re2</t>
+    <t>Ra2</t>
   </si>
   <si>
     <t>Ra3</t>
@@ -446,12 +443,15 @@
     <t>Ra5</t>
   </si>
   <si>
-    <t>5K</t>
+    <t>5.6K</t>
   </si>
   <si>
     <t>Re1</t>
   </si>
   <si>
+    <t>Re2</t>
+  </si>
+  <si>
     <t>Re3</t>
   </si>
   <si>
@@ -476,19 +476,19 @@
     <t>Rf2</t>
   </si>
   <si>
-    <t>100K</t>
+    <t>93.1K</t>
   </si>
   <si>
     <t>Ro1</t>
   </si>
   <si>
-    <t>330K</t>
+    <t>332K +- 1%</t>
   </si>
   <si>
     <t>Ro2</t>
   </si>
   <si>
-    <t>90K</t>
+    <t>90.9K +- 1%</t>
   </si>
   <si>
     <t>58, 60, 62, 64, 66</t>
@@ -497,6 +497,9 @@
     <t>Rq1c, Rq2c, Rq3c, Rq4c, Rq5c</t>
   </si>
   <si>
+    <t>Ru</t>
+  </si>
+  <si>
     <t>RcS</t>
   </si>
   <si>
@@ -654,6 +657,27 @@
   </si>
   <si>
     <t>LM1117LD-3.3/NOPBCT-ND</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>24CW1280T-I/OT</t>
+  </si>
+  <si>
+    <t>EEPROM 128 Kbit I2C</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>579-24CW1280T-I/OT</t>
+  </si>
+  <si>
+    <t>24CW1280T-I/OTCT-ND</t>
   </si>
   <si>
     <t>Y</t>
@@ -707,13 +731,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="mm-dd-yyyy"/>
     <numFmt numFmtId="165" formatCode="d-mmm-yy"/>
     <numFmt numFmtId="166" formatCode="h:mm:ss am/pm"/>
-    <numFmt numFmtId="167" formatCode="m, d"/>
+    <numFmt numFmtId="167" formatCode="m, d, yy"/>
+    <numFmt numFmtId="168" formatCode="m, d"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="35">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -868,6 +893,24 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9.0"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="12.0"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -1416,7 +1459,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="127">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1605,43 +1648,46 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="36" fillId="0" fontId="25" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="20" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="20" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="22" fillId="11" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="23" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="40" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="41" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="40" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="42" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="36" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="20" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="22" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="22" fillId="0" fontId="20" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="22" fillId="11" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="22" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="23" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="40" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="41" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="40" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="42" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="36" fillId="0" fontId="25" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="36" fillId="0" fontId="25" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="22" fillId="12" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -1665,6 +1711,55 @@
     <xf borderId="22" fillId="0" fontId="28" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="22" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="20" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="23" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="40" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="41" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="40" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="42" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="28" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="22" fillId="10" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="41" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="24" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="41" fillId="0" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="43" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -1679,7 +1774,7 @@
     </xf>
     <xf borderId="46" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="47" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="9" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="9" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="14" fillId="10" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1694,7 +1789,7 @@
     <xf borderId="14" fillId="11" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2050,7 +2145,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="33">
-        <v>44028.0</v>
+        <v>44069.0</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="4"/>
@@ -2248,7 +2343,7 @@
     </row>
     <row r="11">
       <c r="A11" s="76">
-        <v>2.0</v>
+        <v>40949.0</v>
       </c>
       <c r="B11" s="77" t="s">
         <v>40</v>
@@ -2302,7 +2397,7 @@
       <c r="AA11" s="75"/>
     </row>
     <row r="12">
-      <c r="A12" s="76">
+      <c r="A12" s="88">
         <v>3.0</v>
       </c>
       <c r="B12" s="77" t="s">
@@ -2357,7 +2452,7 @@
       <c r="AA12" s="75"/>
     </row>
     <row r="13">
-      <c r="A13" s="76">
+      <c r="A13" s="88">
         <v>4.0</v>
       </c>
       <c r="B13" s="77" t="s">
@@ -2412,7 +2507,7 @@
       <c r="AA13" s="75"/>
     </row>
     <row r="14">
-      <c r="A14" s="76">
+      <c r="A14" s="88">
         <v>5.0</v>
       </c>
       <c r="B14" s="77" t="s">
@@ -2467,7 +2562,7 @@
       <c r="AA14" s="75"/>
     </row>
     <row r="15">
-      <c r="A15" s="88">
+      <c r="A15" s="89">
         <v>43995.0</v>
       </c>
       <c r="B15" s="77" t="s">
@@ -2522,7 +2617,7 @@
       <c r="AA15" s="75"/>
     </row>
     <row r="16">
-      <c r="A16" s="76">
+      <c r="A16" s="88">
         <v>7.0</v>
       </c>
       <c r="B16" s="77" t="s">
@@ -2577,7 +2672,7 @@
       <c r="AA16" s="75"/>
     </row>
     <row r="17">
-      <c r="A17" s="88">
+      <c r="A17" s="89">
         <v>44057.0</v>
       </c>
       <c r="B17" s="77" t="s">
@@ -2632,7 +2727,7 @@
       <c r="AA17" s="75"/>
     </row>
     <row r="18">
-      <c r="A18" s="76">
+      <c r="A18" s="88">
         <v>9.0</v>
       </c>
       <c r="B18" s="77" t="s">
@@ -2687,7 +2782,7 @@
       <c r="AA18" s="75"/>
     </row>
     <row r="19">
-      <c r="A19" s="76">
+      <c r="A19" s="88">
         <v>11.0</v>
       </c>
       <c r="B19" s="77" t="s">
@@ -2742,7 +2837,7 @@
       <c r="AA19" s="75"/>
     </row>
     <row r="20">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="88" t="s">
         <v>65</v>
       </c>
       <c r="B20" s="77" t="s">
@@ -2797,7 +2892,7 @@
       <c r="AA20" s="75"/>
     </row>
     <row r="21">
-      <c r="A21" s="76" t="s">
+      <c r="A21" s="88" t="s">
         <v>67</v>
       </c>
       <c r="B21" s="77" t="s">
@@ -2852,7 +2947,7 @@
       <c r="AA21" s="75"/>
     </row>
     <row r="22">
-      <c r="A22" s="76" t="s">
+      <c r="A22" s="88" t="s">
         <v>70</v>
       </c>
       <c r="B22" s="77" t="s">
@@ -2867,7 +2962,7 @@
       <c r="E22" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="89"/>
+      <c r="F22" s="90"/>
       <c r="G22" s="81">
         <v>5.0</v>
       </c>
@@ -2880,7 +2975,7 @@
       <c r="J22" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="K22" s="90" t="s">
+      <c r="K22" s="91" t="s">
         <v>36</v>
       </c>
       <c r="L22" s="85" t="s">
@@ -2907,7 +3002,7 @@
       <c r="AA22" s="75"/>
     </row>
     <row r="23">
-      <c r="A23" s="76">
+      <c r="A23" s="88">
         <v>24.0</v>
       </c>
       <c r="B23" s="77" t="s">
@@ -2919,10 +3014,10 @@
       <c r="D23" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="E23" s="91" t="s">
+      <c r="E23" s="92" t="s">
         <v>80</v>
       </c>
-      <c r="F23" s="89"/>
+      <c r="F23" s="90"/>
       <c r="G23" s="81">
         <v>1.0</v>
       </c>
@@ -2935,7 +3030,7 @@
       <c r="J23" s="78" t="s">
         <v>82</v>
       </c>
-      <c r="K23" s="90" t="s">
+      <c r="K23" s="91" t="s">
         <v>36</v>
       </c>
       <c r="L23" s="83" t="s">
@@ -2944,7 +3039,7 @@
       <c r="M23" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="N23" s="92" t="s">
+      <c r="N23" s="93" t="s">
         <v>39</v>
       </c>
       <c r="O23" s="87"/>
@@ -2962,7 +3057,7 @@
       <c r="AA23" s="75"/>
     </row>
     <row r="24">
-      <c r="A24" s="76">
+      <c r="A24" s="88">
         <v>26.0</v>
       </c>
       <c r="B24" s="77" t="s">
@@ -2974,7 +3069,7 @@
       <c r="D24" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="E24" s="91" t="s">
+      <c r="E24" s="92" t="s">
         <v>87</v>
       </c>
       <c r="F24" s="80"/>
@@ -2990,7 +3085,7 @@
       <c r="J24" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="K24" s="90" t="s">
+      <c r="K24" s="91" t="s">
         <v>36</v>
       </c>
       <c r="L24" s="85" t="s">
@@ -3017,7 +3112,7 @@
       <c r="AA24" s="75"/>
     </row>
     <row r="25">
-      <c r="A25" s="76">
+      <c r="A25" s="88">
         <v>28.0</v>
       </c>
       <c r="B25" s="77" t="s">
@@ -3029,7 +3124,7 @@
       <c r="D25" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="91" t="s">
+      <c r="E25" s="92" t="s">
         <v>87</v>
       </c>
       <c r="F25" s="80"/>
@@ -3045,7 +3140,7 @@
       <c r="J25" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="K25" s="90" t="s">
+      <c r="K25" s="91" t="s">
         <v>36</v>
       </c>
       <c r="L25" s="85" t="s">
@@ -3072,7 +3167,7 @@
       <c r="AA25" s="75"/>
     </row>
     <row r="26">
-      <c r="A26" s="76">
+      <c r="A26" s="88">
         <v>27.0</v>
       </c>
       <c r="B26" s="77" t="s">
@@ -3084,10 +3179,10 @@
       <c r="D26" s="78" t="s">
         <v>96</v>
       </c>
-      <c r="E26" s="93" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" s="94"/>
+      <c r="E26" s="94" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="95"/>
       <c r="G26" s="81">
         <v>1.0</v>
       </c>
@@ -3100,7 +3195,7 @@
       <c r="J26" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="K26" s="90" t="s">
+      <c r="K26" s="91" t="s">
         <v>99</v>
       </c>
       <c r="L26" s="85" t="s">
@@ -3127,7 +3222,7 @@
       <c r="AA26" s="75"/>
     </row>
     <row r="27">
-      <c r="A27" s="76">
+      <c r="A27" s="88">
         <v>29.0</v>
       </c>
       <c r="B27" s="77" t="s">
@@ -3139,10 +3234,10 @@
       <c r="D27" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="E27" s="93" t="s">
-        <v>44</v>
-      </c>
-      <c r="F27" s="94"/>
+      <c r="E27" s="94" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="95"/>
       <c r="G27" s="81">
         <v>1.0</v>
       </c>
@@ -3155,7 +3250,7 @@
       <c r="J27" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="K27" s="90" t="s">
+      <c r="K27" s="91" t="s">
         <v>99</v>
       </c>
       <c r="L27" s="85" t="s">
@@ -3182,7 +3277,7 @@
       <c r="AA27" s="75"/>
     </row>
     <row r="28">
-      <c r="A28" s="76">
+      <c r="A28" s="88">
         <v>30.0</v>
       </c>
       <c r="B28" s="77" t="s">
@@ -3237,7 +3332,7 @@
       <c r="AA28" s="75"/>
     </row>
     <row r="29">
-      <c r="A29" s="76">
+      <c r="A29" s="88">
         <v>31.0</v>
       </c>
       <c r="B29" s="77" t="s">
@@ -3249,7 +3344,7 @@
       <c r="D29" s="78" t="s">
         <v>108</v>
       </c>
-      <c r="E29" s="95" t="s">
+      <c r="E29" s="96" t="s">
         <v>50</v>
       </c>
       <c r="F29" s="80"/>
@@ -3292,7 +3387,7 @@
       <c r="AA29" s="75"/>
     </row>
     <row r="30">
-      <c r="A30" s="76" t="s">
+      <c r="A30" s="88" t="s">
         <v>109</v>
       </c>
       <c r="B30" s="77" t="s">
@@ -3304,10 +3399,10 @@
       <c r="D30" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="E30" s="91" t="s">
+      <c r="E30" s="92" t="s">
         <v>113</v>
       </c>
-      <c r="F30" s="94"/>
+      <c r="F30" s="95"/>
       <c r="G30" s="81">
         <v>2.0</v>
       </c>
@@ -3320,7 +3415,7 @@
       <c r="J30" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="K30" s="90" t="s">
+      <c r="K30" s="91" t="s">
         <v>36</v>
       </c>
       <c r="L30" s="83" t="s">
@@ -3329,7 +3424,7 @@
       <c r="M30" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="N30" s="92" t="s">
+      <c r="N30" s="93" t="s">
         <v>39</v>
       </c>
       <c r="O30" s="87"/>
@@ -3347,7 +3442,7 @@
       <c r="AA30" s="75"/>
     </row>
     <row r="31">
-      <c r="A31" s="76" t="s">
+      <c r="A31" s="88" t="s">
         <v>117</v>
       </c>
       <c r="B31" s="77" t="s">
@@ -3362,7 +3457,7 @@
       <c r="E31" s="79" t="s">
         <v>121</v>
       </c>
-      <c r="F31" s="89" t="s">
+      <c r="F31" s="90" t="s">
         <v>122</v>
       </c>
       <c r="G31" s="81">
@@ -3377,7 +3472,7 @@
       <c r="J31" s="78" t="s">
         <v>124</v>
       </c>
-      <c r="K31" s="90" t="s">
+      <c r="K31" s="91" t="s">
         <v>36</v>
       </c>
       <c r="L31" s="83" t="s">
@@ -3386,7 +3481,7 @@
       <c r="M31" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="N31" s="92" t="s">
+      <c r="N31" s="93" t="s">
         <v>39</v>
       </c>
       <c r="O31" s="87"/>
@@ -3404,7 +3499,7 @@
       <c r="AA31" s="75"/>
     </row>
     <row r="32">
-      <c r="A32" s="76">
+      <c r="A32" s="88">
         <v>39.0</v>
       </c>
       <c r="B32" s="77" t="s">
@@ -3459,11 +3554,11 @@
       <c r="AA32" s="75"/>
     </row>
     <row r="33">
-      <c r="A33" s="76" t="s">
+      <c r="A33" s="88">
+        <v>40.0</v>
+      </c>
+      <c r="B33" s="77" t="s">
         <v>129</v>
-      </c>
-      <c r="B33" s="77" t="s">
-        <v>130</v>
       </c>
       <c r="C33" s="63">
         <v>200.0</v>
@@ -3475,8 +3570,8 @@
         <v>43</v>
       </c>
       <c r="F33" s="80"/>
-      <c r="G33" s="81">
-        <v>2.0</v>
+      <c r="G33" s="97">
+        <v>1.0</v>
       </c>
       <c r="H33" s="82" t="s">
         <v>44</v>
@@ -3514,11 +3609,11 @@
       <c r="AA33" s="75"/>
     </row>
     <row r="34">
-      <c r="A34" s="76">
+      <c r="A34" s="88">
         <v>41.0</v>
       </c>
       <c r="B34" s="77" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C34" s="63">
         <v>499.0</v>
@@ -3569,14 +3664,14 @@
       <c r="AA34" s="75"/>
     </row>
     <row r="35">
-      <c r="A35" s="76" t="s">
+      <c r="A35" s="88" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" s="77" t="s">
         <v>132</v>
       </c>
-      <c r="B35" s="77" t="s">
+      <c r="C35" s="63" t="s">
         <v>133</v>
-      </c>
-      <c r="C35" s="63" t="s">
-        <v>134</v>
       </c>
       <c r="D35" s="78" t="s">
         <v>128</v>
@@ -3624,14 +3719,14 @@
       <c r="AA35" s="75"/>
     </row>
     <row r="36">
-      <c r="A36" s="76">
+      <c r="A36" s="88">
         <v>43.0</v>
       </c>
       <c r="B36" s="77" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" s="98" t="s">
         <v>135</v>
-      </c>
-      <c r="C36" s="63" t="s">
-        <v>136</v>
       </c>
       <c r="D36" s="78" t="s">
         <v>128</v>
@@ -3679,14 +3774,14 @@
       <c r="AA36" s="75"/>
     </row>
     <row r="37">
-      <c r="A37" s="76">
+      <c r="A37" s="88">
         <v>46.0</v>
       </c>
       <c r="B37" s="77" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" s="63">
-        <v>260.0</v>
+        <v>136</v>
+      </c>
+      <c r="C37" s="98">
+        <v>261.0</v>
       </c>
       <c r="D37" s="78" t="s">
         <v>128</v>
@@ -3734,44 +3829,44 @@
       <c r="AA37" s="75"/>
     </row>
     <row r="38">
-      <c r="A38" s="76">
-        <v>48.0</v>
+      <c r="A38" s="88">
+        <v>47.0</v>
       </c>
       <c r="B38" s="77" t="s">
-        <v>138</v>
-      </c>
-      <c r="C38" s="63" t="s">
-        <v>139</v>
-      </c>
-      <c r="D38" s="78" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="98">
+        <v>205.0</v>
+      </c>
+      <c r="D38" s="99" t="s">
         <v>128</v>
       </c>
-      <c r="E38" s="79" t="s">
+      <c r="E38" s="96" t="s">
         <v>43</v>
       </c>
       <c r="F38" s="80"/>
-      <c r="G38" s="81">
+      <c r="G38" s="97">
         <v>1.0</v>
       </c>
-      <c r="H38" s="82" t="s">
-        <v>44</v>
-      </c>
-      <c r="I38" s="83" t="s">
-        <v>44</v>
-      </c>
-      <c r="J38" s="78" t="s">
-        <v>44</v>
-      </c>
-      <c r="K38" s="84" t="s">
-        <v>44</v>
-      </c>
-      <c r="L38" s="85" t="s">
-        <v>44</v>
-      </c>
-      <c r="M38" s="81" t="s">
-        <v>44</v>
-      </c>
-      <c r="N38" s="86" t="s">
+      <c r="H38" s="100" t="s">
+        <v>44</v>
+      </c>
+      <c r="I38" s="101" t="s">
+        <v>44</v>
+      </c>
+      <c r="J38" s="99" t="s">
+        <v>44</v>
+      </c>
+      <c r="K38" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="L38" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="M38" s="97" t="s">
+        <v>44</v>
+      </c>
+      <c r="N38" s="104" t="s">
         <v>44</v>
       </c>
       <c r="O38" s="87"/>
@@ -3789,14 +3884,14 @@
       <c r="AA38" s="75"/>
     </row>
     <row r="39">
-      <c r="A39" s="76" t="s">
-        <v>140</v>
+      <c r="A39" s="88">
+        <v>48.0</v>
       </c>
       <c r="B39" s="77" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C39" s="63" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D39" s="78" t="s">
         <v>128</v>
@@ -3806,7 +3901,7 @@
       </c>
       <c r="F39" s="80"/>
       <c r="G39" s="81">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="H39" s="82" t="s">
         <v>44</v>
@@ -3844,14 +3939,14 @@
       <c r="AA39" s="75"/>
     </row>
     <row r="40">
-      <c r="A40" s="76">
-        <v>51.0</v>
+      <c r="A40" s="88" t="s">
+        <v>140</v>
       </c>
       <c r="B40" s="77" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C40" s="63" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D40" s="78" t="s">
         <v>128</v>
@@ -3861,7 +3956,7 @@
       </c>
       <c r="F40" s="80"/>
       <c r="G40" s="81">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H40" s="82" t="s">
         <v>44</v>
@@ -3899,14 +3994,14 @@
       <c r="AA40" s="75"/>
     </row>
     <row r="41">
-      <c r="A41" s="76">
-        <v>52.0</v>
+      <c r="A41" s="88">
+        <v>51.0</v>
       </c>
       <c r="B41" s="77" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C41" s="63" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D41" s="78" t="s">
         <v>128</v>
@@ -3954,14 +4049,14 @@
       <c r="AA41" s="75"/>
     </row>
     <row r="42">
-      <c r="A42" s="76">
-        <v>53.0</v>
+      <c r="A42" s="88">
+        <v>52.0</v>
       </c>
       <c r="B42" s="77" t="s">
-        <v>147</v>
-      </c>
-      <c r="C42" s="63" t="s">
-        <v>148</v>
+        <v>145</v>
+      </c>
+      <c r="C42" s="98" t="s">
+        <v>146</v>
       </c>
       <c r="D42" s="78" t="s">
         <v>128</v>
@@ -4009,14 +4104,14 @@
       <c r="AA42" s="75"/>
     </row>
     <row r="43">
-      <c r="A43" s="76">
-        <v>54.0</v>
+      <c r="A43" s="88">
+        <v>53.0</v>
       </c>
       <c r="B43" s="77" t="s">
-        <v>149</v>
-      </c>
-      <c r="C43" s="63" t="s">
-        <v>150</v>
+        <v>147</v>
+      </c>
+      <c r="C43" s="98" t="s">
+        <v>148</v>
       </c>
       <c r="D43" s="78" t="s">
         <v>128</v>
@@ -4064,14 +4159,14 @@
       <c r="AA43" s="75"/>
     </row>
     <row r="44">
-      <c r="A44" s="76" t="s">
-        <v>151</v>
+      <c r="A44" s="88">
+        <v>54.0</v>
       </c>
       <c r="B44" s="77" t="s">
-        <v>152</v>
-      </c>
-      <c r="C44" s="63">
-        <v>130.0</v>
+        <v>149</v>
+      </c>
+      <c r="C44" s="98" t="s">
+        <v>150</v>
       </c>
       <c r="D44" s="78" t="s">
         <v>128</v>
@@ -4081,7 +4176,7 @@
       </c>
       <c r="F44" s="80"/>
       <c r="G44" s="81">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="H44" s="82" t="s">
         <v>44</v>
@@ -4119,45 +4214,45 @@
       <c r="AA44" s="75"/>
     </row>
     <row r="45">
-      <c r="A45" s="76">
-        <v>44.0</v>
+      <c r="A45" s="88" t="s">
+        <v>151</v>
       </c>
       <c r="B45" s="77" t="s">
-        <v>153</v>
-      </c>
-      <c r="C45" s="63" t="s">
-        <v>154</v>
+        <v>152</v>
+      </c>
+      <c r="C45" s="63">
+        <v>130.0</v>
       </c>
       <c r="D45" s="78" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="E45" s="79" t="s">
-        <v>156</v>
-      </c>
-      <c r="F45" s="94"/>
+        <v>43</v>
+      </c>
+      <c r="F45" s="80"/>
       <c r="G45" s="81">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H45" s="82" t="s">
-        <v>157</v>
+        <v>44</v>
       </c>
       <c r="I45" s="83" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="J45" s="78" t="s">
-        <v>158</v>
-      </c>
-      <c r="K45" s="90" t="s">
-        <v>36</v>
-      </c>
-      <c r="L45" s="83" t="s">
-        <v>37</v>
-      </c>
-      <c r="M45" s="78" t="s">
-        <v>159</v>
-      </c>
-      <c r="N45" s="92" t="s">
-        <v>39</v>
+        <v>44</v>
+      </c>
+      <c r="K45" s="84" t="s">
+        <v>44</v>
+      </c>
+      <c r="L45" s="85" t="s">
+        <v>44</v>
+      </c>
+      <c r="M45" s="81" t="s">
+        <v>44</v>
+      </c>
+      <c r="N45" s="86" t="s">
+        <v>44</v>
       </c>
       <c r="O45" s="87"/>
       <c r="P45" s="87"/>
@@ -4174,45 +4269,45 @@
       <c r="AA45" s="75"/>
     </row>
     <row r="46">
-      <c r="A46" s="76">
+      <c r="A46" s="88">
         <v>67.0</v>
       </c>
       <c r="B46" s="77" t="s">
-        <v>160</v>
-      </c>
-      <c r="C46" s="63" t="s">
-        <v>161</v>
-      </c>
-      <c r="D46" s="78" t="s">
-        <v>162</v>
-      </c>
-      <c r="E46" s="79" t="s">
-        <v>163</v>
-      </c>
-      <c r="F46" s="94"/>
-      <c r="G46" s="81">
+        <v>153</v>
+      </c>
+      <c r="C46" s="98">
+        <v>10.0</v>
+      </c>
+      <c r="D46" s="99" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" s="96" t="s">
+        <v>43</v>
+      </c>
+      <c r="F46" s="80"/>
+      <c r="G46" s="97">
         <v>1.0</v>
       </c>
-      <c r="H46" s="82" t="s">
-        <v>164</v>
-      </c>
-      <c r="I46" s="83" t="s">
-        <v>34</v>
-      </c>
-      <c r="J46" s="78" t="s">
-        <v>165</v>
-      </c>
-      <c r="K46" s="90" t="s">
-        <v>36</v>
-      </c>
-      <c r="L46" s="83" t="s">
-        <v>37</v>
-      </c>
-      <c r="M46" s="78" t="s">
-        <v>166</v>
-      </c>
-      <c r="N46" s="92" t="s">
-        <v>39</v>
+      <c r="H46" s="100" t="s">
+        <v>44</v>
+      </c>
+      <c r="I46" s="101" t="s">
+        <v>44</v>
+      </c>
+      <c r="J46" s="99" t="s">
+        <v>44</v>
+      </c>
+      <c r="K46" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="L46" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="M46" s="97" t="s">
+        <v>44</v>
+      </c>
+      <c r="N46" s="104" t="s">
+        <v>44</v>
       </c>
       <c r="O46" s="87"/>
       <c r="P46" s="87"/>
@@ -4229,44 +4324,44 @@
       <c r="AA46" s="75"/>
     </row>
     <row r="47">
-      <c r="A47" s="76">
-        <v>68.0</v>
+      <c r="A47" s="88">
+        <v>44.0</v>
       </c>
       <c r="B47" s="77" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="C47" s="63" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="D47" s="78" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="E47" s="79" t="s">
-        <v>170</v>
-      </c>
-      <c r="F47" s="94"/>
+        <v>157</v>
+      </c>
+      <c r="F47" s="95"/>
       <c r="G47" s="81">
         <v>1.0</v>
       </c>
       <c r="H47" s="82" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="I47" s="83" t="s">
         <v>34</v>
       </c>
       <c r="J47" s="78" t="s">
-        <v>172</v>
-      </c>
-      <c r="K47" s="90" t="s">
+        <v>159</v>
+      </c>
+      <c r="K47" s="91" t="s">
         <v>36</v>
       </c>
       <c r="L47" s="83" t="s">
         <v>37</v>
       </c>
       <c r="M47" s="78" t="s">
-        <v>173</v>
-      </c>
-      <c r="N47" s="92" t="s">
+        <v>160</v>
+      </c>
+      <c r="N47" s="93" t="s">
         <v>39</v>
       </c>
       <c r="O47" s="87"/>
@@ -4284,44 +4379,44 @@
       <c r="AA47" s="75"/>
     </row>
     <row r="48">
-      <c r="A48" s="76">
-        <v>69.0</v>
+      <c r="A48" s="88">
+        <v>68.0</v>
       </c>
       <c r="B48" s="77" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="C48" s="63" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="D48" s="78" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="E48" s="79" t="s">
-        <v>177</v>
-      </c>
-      <c r="F48" s="94"/>
+        <v>164</v>
+      </c>
+      <c r="F48" s="95"/>
       <c r="G48" s="81">
         <v>1.0</v>
       </c>
       <c r="H48" s="82" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="I48" s="83" t="s">
         <v>34</v>
       </c>
       <c r="J48" s="78" t="s">
-        <v>179</v>
-      </c>
-      <c r="K48" s="90" t="s">
+        <v>166</v>
+      </c>
+      <c r="K48" s="91" t="s">
         <v>36</v>
       </c>
       <c r="L48" s="83" t="s">
         <v>37</v>
       </c>
       <c r="M48" s="78" t="s">
-        <v>180</v>
-      </c>
-      <c r="N48" s="92" t="s">
+        <v>167</v>
+      </c>
+      <c r="N48" s="93" t="s">
         <v>39</v>
       </c>
       <c r="O48" s="87"/>
@@ -4339,45 +4434,45 @@
       <c r="AA48" s="75"/>
     </row>
     <row r="49">
-      <c r="A49" s="76">
-        <v>70.0</v>
+      <c r="A49" s="88">
+        <v>69.0</v>
       </c>
       <c r="B49" s="77" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="C49" s="63" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D49" s="78" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="E49" s="79" t="s">
-        <v>184</v>
-      </c>
-      <c r="F49" s="94"/>
+        <v>171</v>
+      </c>
+      <c r="F49" s="95"/>
       <c r="G49" s="81">
         <v>1.0</v>
       </c>
       <c r="H49" s="82" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="I49" s="83" t="s">
+        <v>34</v>
+      </c>
+      <c r="J49" s="78" t="s">
+        <v>173</v>
+      </c>
+      <c r="K49" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="L49" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="J49" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="K49" s="90" t="s">
+      <c r="M49" s="78" t="s">
+        <v>174</v>
+      </c>
+      <c r="N49" s="93" t="s">
         <v>39</v>
-      </c>
-      <c r="L49" s="83" t="s">
-        <v>34</v>
-      </c>
-      <c r="M49" s="78" t="s">
-        <v>187</v>
-      </c>
-      <c r="N49" s="92" t="s">
-        <v>36</v>
       </c>
       <c r="O49" s="87"/>
       <c r="P49" s="87"/>
@@ -4394,44 +4489,44 @@
       <c r="AA49" s="75"/>
     </row>
     <row r="50">
-      <c r="A50" s="76">
-        <v>71.0</v>
+      <c r="A50" s="88">
+        <v>70.0</v>
       </c>
       <c r="B50" s="77" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C50" s="63" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="D50" s="78" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="E50" s="79" t="s">
-        <v>191</v>
-      </c>
-      <c r="F50" s="94"/>
+        <v>178</v>
+      </c>
+      <c r="F50" s="95"/>
       <c r="G50" s="81">
         <v>1.0</v>
       </c>
       <c r="H50" s="82" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I50" s="83" t="s">
         <v>34</v>
       </c>
       <c r="J50" s="78" t="s">
-        <v>192</v>
-      </c>
-      <c r="K50" s="90" t="s">
+        <v>180</v>
+      </c>
+      <c r="K50" s="91" t="s">
         <v>36</v>
       </c>
       <c r="L50" s="83" t="s">
         <v>37</v>
       </c>
       <c r="M50" s="78" t="s">
-        <v>193</v>
-      </c>
-      <c r="N50" s="92" t="s">
+        <v>181</v>
+      </c>
+      <c r="N50" s="93" t="s">
         <v>39</v>
       </c>
       <c r="O50" s="87"/>
@@ -4449,45 +4544,45 @@
       <c r="AA50" s="75"/>
     </row>
     <row r="51">
-      <c r="A51" s="76">
-        <v>72.0</v>
+      <c r="A51" s="88">
+        <v>71.0</v>
       </c>
       <c r="B51" s="77" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="C51" s="63" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="D51" s="78" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="E51" s="79" t="s">
-        <v>197</v>
-      </c>
-      <c r="F51" s="94"/>
+        <v>185</v>
+      </c>
+      <c r="F51" s="95"/>
       <c r="G51" s="81">
         <v>1.0</v>
       </c>
       <c r="H51" s="82" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="I51" s="83" t="s">
+        <v>37</v>
+      </c>
+      <c r="J51" s="78" t="s">
+        <v>187</v>
+      </c>
+      <c r="K51" s="91" t="s">
+        <v>39</v>
+      </c>
+      <c r="L51" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="J51" s="78" t="s">
-        <v>198</v>
-      </c>
-      <c r="K51" s="90" t="s">
+      <c r="M51" s="78" t="s">
+        <v>188</v>
+      </c>
+      <c r="N51" s="93" t="s">
         <v>36</v>
-      </c>
-      <c r="L51" s="83" t="s">
-        <v>37</v>
-      </c>
-      <c r="M51" s="78" t="s">
-        <v>199</v>
-      </c>
-      <c r="N51" s="92" t="s">
-        <v>39</v>
       </c>
       <c r="O51" s="87"/>
       <c r="P51" s="87"/>
@@ -4504,44 +4599,44 @@
       <c r="AA51" s="75"/>
     </row>
     <row r="52">
-      <c r="A52" s="76">
-        <v>73.0</v>
+      <c r="A52" s="88">
+        <v>72.0</v>
       </c>
       <c r="B52" s="77" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="C52" s="63" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D52" s="78" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="E52" s="79" t="s">
-        <v>203</v>
-      </c>
-      <c r="F52" s="94"/>
+        <v>192</v>
+      </c>
+      <c r="F52" s="95"/>
       <c r="G52" s="81">
         <v>1.0</v>
       </c>
       <c r="H52" s="82" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I52" s="83" t="s">
         <v>34</v>
       </c>
       <c r="J52" s="78" t="s">
-        <v>204</v>
-      </c>
-      <c r="K52" s="90" t="s">
+        <v>193</v>
+      </c>
+      <c r="K52" s="91" t="s">
         <v>36</v>
       </c>
       <c r="L52" s="83" t="s">
         <v>37</v>
       </c>
       <c r="M52" s="78" t="s">
-        <v>205</v>
-      </c>
-      <c r="N52" s="92" t="s">
+        <v>194</v>
+      </c>
+      <c r="N52" s="93" t="s">
         <v>39</v>
       </c>
       <c r="O52" s="87"/>
@@ -4559,45 +4654,45 @@
       <c r="AA52" s="75"/>
     </row>
     <row r="53">
-      <c r="A53" s="76">
-        <v>74.0</v>
+      <c r="A53" s="88">
+        <v>73.0</v>
       </c>
       <c r="B53" s="77" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C53" s="63" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="D53" s="78" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="E53" s="79" t="s">
-        <v>209</v>
-      </c>
-      <c r="F53" s="89"/>
+        <v>198</v>
+      </c>
+      <c r="F53" s="95"/>
       <c r="G53" s="81">
         <v>1.0</v>
       </c>
       <c r="H53" s="82" t="s">
-        <v>210</v>
+        <v>179</v>
       </c>
       <c r="I53" s="83" t="s">
         <v>34</v>
       </c>
       <c r="J53" s="78" t="s">
-        <v>211</v>
-      </c>
-      <c r="K53" s="90" t="s">
+        <v>199</v>
+      </c>
+      <c r="K53" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="L53" s="85" t="s">
-        <v>44</v>
-      </c>
-      <c r="M53" s="81" t="s">
-        <v>44</v>
-      </c>
-      <c r="N53" s="86" t="s">
-        <v>44</v>
+      <c r="L53" s="83" t="s">
+        <v>37</v>
+      </c>
+      <c r="M53" s="78" t="s">
+        <v>200</v>
+      </c>
+      <c r="N53" s="93" t="s">
+        <v>39</v>
       </c>
       <c r="O53" s="87"/>
       <c r="P53" s="87"/>
@@ -4614,28 +4709,46 @@
       <c r="AA53" s="75"/>
     </row>
     <row r="54">
-      <c r="A54" s="96">
-        <v>25.0</v>
-      </c>
-      <c r="B54" s="97" t="s">
-        <v>212</v>
-      </c>
-      <c r="C54" s="98" t="s">
-        <v>213</v>
-      </c>
-      <c r="D54" s="99" t="s">
-        <v>214</v>
-      </c>
-      <c r="E54" s="100"/>
-      <c r="F54" s="100"/>
-      <c r="G54" s="100"/>
-      <c r="H54" s="100"/>
-      <c r="I54" s="100"/>
-      <c r="J54" s="100"/>
-      <c r="K54" s="100"/>
-      <c r="L54" s="100"/>
-      <c r="M54" s="100"/>
-      <c r="N54" s="101"/>
+      <c r="A54" s="88">
+        <v>74.0</v>
+      </c>
+      <c r="B54" s="77" t="s">
+        <v>201</v>
+      </c>
+      <c r="C54" s="63" t="s">
+        <v>202</v>
+      </c>
+      <c r="D54" s="78" t="s">
+        <v>203</v>
+      </c>
+      <c r="E54" s="79" t="s">
+        <v>204</v>
+      </c>
+      <c r="F54" s="95"/>
+      <c r="G54" s="81">
+        <v>1.0</v>
+      </c>
+      <c r="H54" s="82" t="s">
+        <v>179</v>
+      </c>
+      <c r="I54" s="83" t="s">
+        <v>34</v>
+      </c>
+      <c r="J54" s="78" t="s">
+        <v>205</v>
+      </c>
+      <c r="K54" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="L54" s="83" t="s">
+        <v>37</v>
+      </c>
+      <c r="M54" s="78" t="s">
+        <v>206</v>
+      </c>
+      <c r="N54" s="93" t="s">
+        <v>39</v>
+      </c>
       <c r="O54" s="87"/>
       <c r="P54" s="87"/>
       <c r="Q54" s="87"/>
@@ -4651,59 +4764,107 @@
       <c r="AA54" s="75"/>
     </row>
     <row r="55">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="87"/>
-      <c r="P55" s="87"/>
-      <c r="Q55" s="87"/>
-      <c r="R55" s="87"/>
-      <c r="S55" s="74"/>
-      <c r="T55" s="74"/>
-      <c r="U55" s="74"/>
-      <c r="V55" s="74"/>
-      <c r="W55" s="74"/>
-      <c r="X55" s="75"/>
-      <c r="Y55" s="75"/>
-      <c r="Z55" s="75"/>
-      <c r="AA55" s="75"/>
+      <c r="A55" s="88">
+        <v>75.0</v>
+      </c>
+      <c r="B55" s="105" t="s">
+        <v>207</v>
+      </c>
+      <c r="C55" s="98" t="s">
+        <v>208</v>
+      </c>
+      <c r="D55" s="99" t="s">
+        <v>209</v>
+      </c>
+      <c r="E55" s="106" t="s">
+        <v>210</v>
+      </c>
+      <c r="F55" s="107"/>
+      <c r="G55" s="108">
+        <v>1.0</v>
+      </c>
+      <c r="H55" s="109" t="s">
+        <v>211</v>
+      </c>
+      <c r="I55" s="110" t="s">
+        <v>34</v>
+      </c>
+      <c r="J55" s="111" t="s">
+        <v>212</v>
+      </c>
+      <c r="K55" s="112" t="s">
+        <v>36</v>
+      </c>
+      <c r="L55" s="110" t="s">
+        <v>37</v>
+      </c>
+      <c r="M55" s="111" t="s">
+        <v>213</v>
+      </c>
+      <c r="N55" s="112" t="s">
+        <v>39</v>
+      </c>
+      <c r="O55" s="113"/>
+      <c r="P55" s="113"/>
+      <c r="Q55" s="113"/>
+      <c r="R55" s="113"/>
+      <c r="S55" s="113"/>
+      <c r="T55" s="113"/>
+      <c r="U55" s="113"/>
+      <c r="V55" s="113"/>
+      <c r="W55" s="113"/>
+      <c r="X55" s="113"/>
+      <c r="Y55" s="113"/>
+      <c r="Z55" s="113"/>
+      <c r="AA55" s="113"/>
     </row>
     <row r="56">
-      <c r="A56" s="102" t="s">
+      <c r="A56" s="88">
+        <v>76.0</v>
+      </c>
+      <c r="B56" s="77" t="s">
+        <v>214</v>
+      </c>
+      <c r="C56" s="63" t="s">
         <v>215</v>
       </c>
-      <c r="B56" s="15"/>
-      <c r="C56" s="103"/>
-      <c r="D56" s="104" t="s">
+      <c r="D56" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="E56" s="37"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
-      <c r="N56" s="4"/>
+      <c r="E56" s="79" t="s">
+        <v>217</v>
+      </c>
+      <c r="F56" s="90"/>
+      <c r="G56" s="81">
+        <v>1.0</v>
+      </c>
+      <c r="H56" s="82" t="s">
+        <v>218</v>
+      </c>
+      <c r="I56" s="83" t="s">
+        <v>34</v>
+      </c>
+      <c r="J56" s="78" t="s">
+        <v>219</v>
+      </c>
+      <c r="K56" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="L56" s="85" t="s">
+        <v>44</v>
+      </c>
+      <c r="M56" s="81" t="s">
+        <v>44</v>
+      </c>
+      <c r="N56" s="86" t="s">
+        <v>44</v>
+      </c>
       <c r="O56" s="87"/>
       <c r="P56" s="87"/>
       <c r="Q56" s="87"/>
       <c r="R56" s="87"/>
-      <c r="S56" s="87"/>
-      <c r="T56" s="87"/>
+      <c r="S56" s="74"/>
+      <c r="T56" s="74"/>
       <c r="U56" s="74"/>
       <c r="V56" s="74"/>
       <c r="W56" s="74"/>
@@ -4713,28 +4874,34 @@
       <c r="AA56" s="75"/>
     </row>
     <row r="57">
-      <c r="A57" s="22"/>
-      <c r="B57" s="23"/>
-      <c r="C57" s="105"/>
-      <c r="D57" s="104" t="s">
-        <v>217</v>
-      </c>
-      <c r="E57" s="37"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-      <c r="N57" s="4"/>
+      <c r="A57" s="114">
+        <v>25.0</v>
+      </c>
+      <c r="B57" s="115" t="s">
+        <v>220</v>
+      </c>
+      <c r="C57" s="116" t="s">
+        <v>221</v>
+      </c>
+      <c r="D57" s="117" t="s">
+        <v>222</v>
+      </c>
+      <c r="E57" s="118"/>
+      <c r="F57" s="118"/>
+      <c r="G57" s="118"/>
+      <c r="H57" s="118"/>
+      <c r="I57" s="118"/>
+      <c r="J57" s="118"/>
+      <c r="K57" s="118"/>
+      <c r="L57" s="118"/>
+      <c r="M57" s="118"/>
+      <c r="N57" s="119"/>
       <c r="O57" s="87"/>
       <c r="P57" s="87"/>
       <c r="Q57" s="87"/>
       <c r="R57" s="87"/>
-      <c r="S57" s="87"/>
-      <c r="T57" s="87"/>
+      <c r="S57" s="74"/>
+      <c r="T57" s="74"/>
       <c r="U57" s="74"/>
       <c r="V57" s="74"/>
       <c r="W57" s="74"/>
@@ -4744,14 +4911,12 @@
       <c r="AA57" s="75"/>
     </row>
     <row r="58">
-      <c r="A58" s="30"/>
-      <c r="B58" s="31"/>
-      <c r="C58" s="106"/>
-      <c r="D58" s="104" t="s">
-        <v>218</v>
-      </c>
-      <c r="E58" s="37"/>
-      <c r="F58" s="13"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
@@ -4764,8 +4929,8 @@
       <c r="P58" s="87"/>
       <c r="Q58" s="87"/>
       <c r="R58" s="87"/>
-      <c r="S58" s="87"/>
-      <c r="T58" s="87"/>
+      <c r="S58" s="74"/>
+      <c r="T58" s="74"/>
       <c r="U58" s="74"/>
       <c r="V58" s="74"/>
       <c r="W58" s="74"/>
@@ -4775,12 +4940,16 @@
       <c r="AA58" s="75"/>
     </row>
     <row r="59">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
+      <c r="A59" s="120" t="s">
+        <v>223</v>
+      </c>
+      <c r="B59" s="15"/>
+      <c r="C59" s="121"/>
+      <c r="D59" s="122" t="s">
+        <v>224</v>
+      </c>
+      <c r="E59" s="37"/>
+      <c r="F59" s="13"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -4793,8 +4962,8 @@
       <c r="P59" s="87"/>
       <c r="Q59" s="87"/>
       <c r="R59" s="87"/>
-      <c r="S59" s="74"/>
-      <c r="T59" s="74"/>
+      <c r="S59" s="87"/>
+      <c r="T59" s="87"/>
       <c r="U59" s="74"/>
       <c r="V59" s="74"/>
       <c r="W59" s="74"/>
@@ -4804,26 +4973,28 @@
       <c r="AA59" s="75"/>
     </row>
     <row r="60">
-      <c r="A60" s="107"/>
-      <c r="B60" s="107"/>
-      <c r="C60" s="107"/>
-      <c r="D60" s="107"/>
-      <c r="E60" s="107"/>
-      <c r="F60" s="107"/>
-      <c r="G60" s="107"/>
-      <c r="H60" s="107"/>
-      <c r="I60" s="87"/>
-      <c r="J60" s="87"/>
-      <c r="K60" s="87"/>
-      <c r="L60" s="87"/>
-      <c r="M60" s="87"/>
-      <c r="N60" s="87"/>
+      <c r="A60" s="22"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="123"/>
+      <c r="D60" s="122" t="s">
+        <v>225</v>
+      </c>
+      <c r="E60" s="37"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
       <c r="O60" s="87"/>
       <c r="P60" s="87"/>
       <c r="Q60" s="87"/>
       <c r="R60" s="87"/>
-      <c r="S60" s="74"/>
-      <c r="T60" s="74"/>
+      <c r="S60" s="87"/>
+      <c r="T60" s="87"/>
       <c r="U60" s="74"/>
       <c r="V60" s="74"/>
       <c r="W60" s="74"/>
@@ -4833,244 +5004,333 @@
       <c r="AA60" s="75"/>
     </row>
     <row r="61">
-      <c r="A61" s="108"/>
-      <c r="B61" s="108"/>
-      <c r="C61" s="108"/>
-      <c r="D61" s="108"/>
-      <c r="E61" s="108"/>
-      <c r="F61" s="108"/>
-      <c r="G61" s="108"/>
-      <c r="H61" s="108"/>
-      <c r="I61" s="108"/>
-      <c r="J61" s="108"/>
-      <c r="K61" s="108"/>
-      <c r="L61" s="108"/>
-      <c r="M61" s="108"/>
-      <c r="N61" s="108"/>
-      <c r="O61" s="108"/>
-      <c r="P61" s="108"/>
-      <c r="Q61" s="108"/>
-      <c r="R61" s="108"/>
+      <c r="A61" s="30"/>
+      <c r="B61" s="31"/>
+      <c r="C61" s="124"/>
+      <c r="D61" s="122" t="s">
+        <v>226</v>
+      </c>
+      <c r="E61" s="37"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="87"/>
+      <c r="P61" s="87"/>
+      <c r="Q61" s="87"/>
+      <c r="R61" s="87"/>
+      <c r="S61" s="87"/>
+      <c r="T61" s="87"/>
+      <c r="U61" s="74"/>
+      <c r="V61" s="74"/>
+      <c r="W61" s="74"/>
+      <c r="X61" s="75"/>
+      <c r="Y61" s="75"/>
+      <c r="Z61" s="75"/>
+      <c r="AA61" s="75"/>
     </row>
     <row r="62">
-      <c r="A62" s="108"/>
-      <c r="B62" s="108"/>
-      <c r="C62" s="108"/>
-      <c r="D62" s="108"/>
-      <c r="E62" s="108"/>
-      <c r="F62" s="108"/>
-      <c r="G62" s="108"/>
-      <c r="H62" s="108"/>
-      <c r="I62" s="108"/>
-      <c r="J62" s="108"/>
-      <c r="K62" s="108"/>
-      <c r="L62" s="108"/>
-      <c r="M62" s="108"/>
-      <c r="N62" s="108"/>
-      <c r="O62" s="108"/>
-      <c r="P62" s="108"/>
-      <c r="Q62" s="108"/>
-      <c r="R62" s="108"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="87"/>
+      <c r="P62" s="87"/>
+      <c r="Q62" s="87"/>
+      <c r="R62" s="87"/>
+      <c r="S62" s="74"/>
+      <c r="T62" s="74"/>
+      <c r="U62" s="74"/>
+      <c r="V62" s="74"/>
+      <c r="W62" s="74"/>
+      <c r="X62" s="75"/>
+      <c r="Y62" s="75"/>
+      <c r="Z62" s="75"/>
+      <c r="AA62" s="75"/>
     </row>
     <row r="63">
-      <c r="A63" s="108"/>
-      <c r="B63" s="108"/>
-      <c r="C63" s="108"/>
-      <c r="D63" s="108"/>
-      <c r="E63" s="108"/>
-      <c r="F63" s="108"/>
-      <c r="G63" s="108"/>
-      <c r="H63" s="108"/>
-      <c r="I63" s="108"/>
-      <c r="J63" s="108"/>
-      <c r="K63" s="108"/>
-      <c r="L63" s="108"/>
-      <c r="M63" s="108"/>
-      <c r="N63" s="108"/>
-      <c r="O63" s="108"/>
-      <c r="P63" s="108"/>
-      <c r="Q63" s="108"/>
-      <c r="R63" s="108"/>
+      <c r="A63" s="125"/>
+      <c r="B63" s="125"/>
+      <c r="C63" s="125"/>
+      <c r="D63" s="125"/>
+      <c r="E63" s="125"/>
+      <c r="F63" s="125"/>
+      <c r="G63" s="125"/>
+      <c r="H63" s="125"/>
+      <c r="I63" s="87"/>
+      <c r="J63" s="87"/>
+      <c r="K63" s="87"/>
+      <c r="L63" s="87"/>
+      <c r="M63" s="87"/>
+      <c r="N63" s="87"/>
+      <c r="O63" s="87"/>
+      <c r="P63" s="87"/>
+      <c r="Q63" s="87"/>
+      <c r="R63" s="87"/>
+      <c r="S63" s="74"/>
+      <c r="T63" s="74"/>
+      <c r="U63" s="74"/>
+      <c r="V63" s="74"/>
+      <c r="W63" s="74"/>
+      <c r="X63" s="75"/>
+      <c r="Y63" s="75"/>
+      <c r="Z63" s="75"/>
+      <c r="AA63" s="75"/>
     </row>
     <row r="64">
-      <c r="A64" s="108"/>
-      <c r="B64" s="108"/>
-      <c r="C64" s="108"/>
-      <c r="D64" s="108"/>
-      <c r="E64" s="108"/>
-      <c r="F64" s="108"/>
-      <c r="G64" s="108"/>
-      <c r="H64" s="108"/>
-      <c r="I64" s="108"/>
-      <c r="J64" s="108"/>
-      <c r="K64" s="108"/>
-      <c r="L64" s="108"/>
-      <c r="M64" s="108"/>
-      <c r="N64" s="108"/>
-      <c r="O64" s="108"/>
-      <c r="P64" s="108"/>
-      <c r="Q64" s="108"/>
-      <c r="R64" s="108"/>
+      <c r="A64" s="126"/>
+      <c r="B64" s="126"/>
+      <c r="C64" s="126"/>
+      <c r="D64" s="126"/>
+      <c r="E64" s="126"/>
+      <c r="F64" s="126"/>
+      <c r="G64" s="126"/>
+      <c r="H64" s="126"/>
+      <c r="I64" s="126"/>
+      <c r="J64" s="126"/>
+      <c r="K64" s="126"/>
+      <c r="L64" s="126"/>
+      <c r="M64" s="126"/>
+      <c r="N64" s="126"/>
+      <c r="O64" s="126"/>
+      <c r="P64" s="126"/>
+      <c r="Q64" s="126"/>
+      <c r="R64" s="126"/>
     </row>
     <row r="65">
-      <c r="A65" s="108"/>
-      <c r="B65" s="108"/>
-      <c r="C65" s="108"/>
-      <c r="D65" s="108"/>
-      <c r="E65" s="108"/>
-      <c r="F65" s="108"/>
-      <c r="G65" s="108"/>
-      <c r="H65" s="108"/>
-      <c r="I65" s="108"/>
-      <c r="J65" s="108"/>
-      <c r="K65" s="108"/>
-      <c r="L65" s="108"/>
-      <c r="M65" s="108"/>
-      <c r="N65" s="108"/>
-      <c r="O65" s="108"/>
-      <c r="P65" s="108"/>
-      <c r="Q65" s="108"/>
-      <c r="R65" s="108"/>
+      <c r="A65" s="126"/>
+      <c r="B65" s="126"/>
+      <c r="C65" s="126"/>
+      <c r="D65" s="126"/>
+      <c r="E65" s="126"/>
+      <c r="F65" s="126"/>
+      <c r="G65" s="126"/>
+      <c r="H65" s="126"/>
+      <c r="I65" s="126"/>
+      <c r="J65" s="126"/>
+      <c r="K65" s="126"/>
+      <c r="L65" s="126"/>
+      <c r="M65" s="126"/>
+      <c r="N65" s="126"/>
+      <c r="O65" s="126"/>
+      <c r="P65" s="126"/>
+      <c r="Q65" s="126"/>
+      <c r="R65" s="126"/>
     </row>
     <row r="66">
-      <c r="A66" s="108"/>
-      <c r="B66" s="108"/>
-      <c r="C66" s="108"/>
-      <c r="D66" s="108"/>
-      <c r="E66" s="108"/>
-      <c r="F66" s="108"/>
-      <c r="G66" s="108"/>
-      <c r="H66" s="108"/>
-      <c r="I66" s="108"/>
-      <c r="J66" s="108"/>
-      <c r="K66" s="108"/>
-      <c r="L66" s="108"/>
-      <c r="M66" s="108"/>
-      <c r="N66" s="108"/>
-      <c r="O66" s="108"/>
-      <c r="P66" s="108"/>
-      <c r="Q66" s="108"/>
-      <c r="R66" s="108"/>
+      <c r="A66" s="126"/>
+      <c r="B66" s="126"/>
+      <c r="C66" s="126"/>
+      <c r="D66" s="126"/>
+      <c r="E66" s="126"/>
+      <c r="F66" s="126"/>
+      <c r="G66" s="126"/>
+      <c r="H66" s="126"/>
+      <c r="I66" s="126"/>
+      <c r="J66" s="126"/>
+      <c r="K66" s="126"/>
+      <c r="L66" s="126"/>
+      <c r="M66" s="126"/>
+      <c r="N66" s="126"/>
+      <c r="O66" s="126"/>
+      <c r="P66" s="126"/>
+      <c r="Q66" s="126"/>
+      <c r="R66" s="126"/>
     </row>
     <row r="67">
-      <c r="A67" s="108"/>
-      <c r="B67" s="108"/>
-      <c r="C67" s="108"/>
-      <c r="D67" s="108"/>
-      <c r="E67" s="108"/>
-      <c r="F67" s="108"/>
-      <c r="G67" s="108"/>
-      <c r="H67" s="108"/>
-      <c r="I67" s="108"/>
-      <c r="J67" s="108"/>
-      <c r="K67" s="108"/>
-      <c r="L67" s="108"/>
-      <c r="M67" s="108"/>
-      <c r="N67" s="108"/>
-      <c r="O67" s="108"/>
-      <c r="P67" s="108"/>
-      <c r="Q67" s="108"/>
-      <c r="R67" s="108"/>
+      <c r="A67" s="126"/>
+      <c r="B67" s="126"/>
+      <c r="C67" s="126"/>
+      <c r="D67" s="126"/>
+      <c r="E67" s="126"/>
+      <c r="F67" s="126"/>
+      <c r="G67" s="126"/>
+      <c r="H67" s="126"/>
+      <c r="I67" s="126"/>
+      <c r="J67" s="126"/>
+      <c r="K67" s="126"/>
+      <c r="L67" s="126"/>
+      <c r="M67" s="126"/>
+      <c r="N67" s="126"/>
+      <c r="O67" s="126"/>
+      <c r="P67" s="126"/>
+      <c r="Q67" s="126"/>
+      <c r="R67" s="126"/>
     </row>
     <row r="68">
-      <c r="A68" s="108"/>
-      <c r="B68" s="108"/>
-      <c r="C68" s="108"/>
-      <c r="D68" s="108"/>
-      <c r="E68" s="108"/>
-      <c r="F68" s="108"/>
-      <c r="G68" s="108"/>
-      <c r="H68" s="108"/>
-      <c r="I68" s="108"/>
-      <c r="J68" s="108"/>
-      <c r="K68" s="108"/>
-      <c r="L68" s="108"/>
-      <c r="M68" s="108"/>
-      <c r="N68" s="108"/>
-      <c r="O68" s="108"/>
-      <c r="P68" s="108"/>
-      <c r="Q68" s="108"/>
-      <c r="R68" s="108"/>
+      <c r="A68" s="126"/>
+      <c r="B68" s="126"/>
+      <c r="C68" s="126"/>
+      <c r="D68" s="126"/>
+      <c r="E68" s="126"/>
+      <c r="F68" s="126"/>
+      <c r="G68" s="126"/>
+      <c r="H68" s="126"/>
+      <c r="I68" s="126"/>
+      <c r="J68" s="126"/>
+      <c r="K68" s="126"/>
+      <c r="L68" s="126"/>
+      <c r="M68" s="126"/>
+      <c r="N68" s="126"/>
+      <c r="O68" s="126"/>
+      <c r="P68" s="126"/>
+      <c r="Q68" s="126"/>
+      <c r="R68" s="126"/>
     </row>
     <row r="69">
-      <c r="A69" s="108"/>
-      <c r="B69" s="108"/>
-      <c r="C69" s="108"/>
-      <c r="D69" s="108"/>
-      <c r="E69" s="108"/>
-      <c r="F69" s="108"/>
-      <c r="G69" s="108"/>
-      <c r="H69" s="108"/>
-      <c r="I69" s="108"/>
-      <c r="J69" s="108"/>
-      <c r="K69" s="108"/>
-      <c r="L69" s="108"/>
-      <c r="M69" s="108"/>
-      <c r="N69" s="108"/>
-      <c r="O69" s="108"/>
-      <c r="P69" s="108"/>
-      <c r="Q69" s="108"/>
-      <c r="R69" s="108"/>
+      <c r="A69" s="126"/>
+      <c r="B69" s="126"/>
+      <c r="C69" s="126"/>
+      <c r="D69" s="126"/>
+      <c r="E69" s="126"/>
+      <c r="F69" s="126"/>
+      <c r="G69" s="126"/>
+      <c r="H69" s="126"/>
+      <c r="I69" s="126"/>
+      <c r="J69" s="126"/>
+      <c r="K69" s="126"/>
+      <c r="L69" s="126"/>
+      <c r="M69" s="126"/>
+      <c r="N69" s="126"/>
+      <c r="O69" s="126"/>
+      <c r="P69" s="126"/>
+      <c r="Q69" s="126"/>
+      <c r="R69" s="126"/>
     </row>
     <row r="70">
-      <c r="A70" s="108"/>
-      <c r="B70" s="108"/>
-      <c r="C70" s="108"/>
-      <c r="D70" s="108"/>
-      <c r="E70" s="108"/>
-      <c r="F70" s="108"/>
-      <c r="G70" s="108"/>
-      <c r="H70" s="108"/>
-      <c r="I70" s="108"/>
-      <c r="J70" s="108"/>
-      <c r="K70" s="108"/>
-      <c r="L70" s="108"/>
-      <c r="M70" s="108"/>
-      <c r="N70" s="108"/>
-      <c r="O70" s="108"/>
-      <c r="P70" s="108"/>
-      <c r="Q70" s="108"/>
-      <c r="R70" s="108"/>
+      <c r="A70" s="126"/>
+      <c r="B70" s="126"/>
+      <c r="C70" s="126"/>
+      <c r="D70" s="126"/>
+      <c r="E70" s="126"/>
+      <c r="F70" s="126"/>
+      <c r="G70" s="126"/>
+      <c r="H70" s="126"/>
+      <c r="I70" s="126"/>
+      <c r="J70" s="126"/>
+      <c r="K70" s="126"/>
+      <c r="L70" s="126"/>
+      <c r="M70" s="126"/>
+      <c r="N70" s="126"/>
+      <c r="O70" s="126"/>
+      <c r="P70" s="126"/>
+      <c r="Q70" s="126"/>
+      <c r="R70" s="126"/>
     </row>
     <row r="71">
-      <c r="A71" s="108"/>
-      <c r="B71" s="108"/>
-      <c r="C71" s="108"/>
-      <c r="D71" s="108"/>
-      <c r="E71" s="108"/>
-      <c r="F71" s="108"/>
-      <c r="G71" s="108"/>
-      <c r="H71" s="108"/>
-      <c r="I71" s="108"/>
-      <c r="J71" s="108"/>
-      <c r="K71" s="108"/>
-      <c r="L71" s="108"/>
-      <c r="M71" s="108"/>
-      <c r="N71" s="108"/>
-      <c r="O71" s="108"/>
-      <c r="P71" s="108"/>
-      <c r="Q71" s="108"/>
-      <c r="R71" s="108"/>
+      <c r="A71" s="126"/>
+      <c r="B71" s="126"/>
+      <c r="C71" s="126"/>
+      <c r="D71" s="126"/>
+      <c r="E71" s="126"/>
+      <c r="F71" s="126"/>
+      <c r="G71" s="126"/>
+      <c r="H71" s="126"/>
+      <c r="I71" s="126"/>
+      <c r="J71" s="126"/>
+      <c r="K71" s="126"/>
+      <c r="L71" s="126"/>
+      <c r="M71" s="126"/>
+      <c r="N71" s="126"/>
+      <c r="O71" s="126"/>
+      <c r="P71" s="126"/>
+      <c r="Q71" s="126"/>
+      <c r="R71" s="126"/>
     </row>
     <row r="72">
-      <c r="A72" s="108"/>
-      <c r="B72" s="108"/>
-      <c r="C72" s="108"/>
-      <c r="D72" s="108"/>
-      <c r="E72" s="108"/>
-      <c r="F72" s="108"/>
-      <c r="G72" s="108"/>
-      <c r="H72" s="108"/>
-      <c r="I72" s="108"/>
-      <c r="J72" s="108"/>
-      <c r="K72" s="108"/>
-      <c r="L72" s="108"/>
-      <c r="M72" s="108"/>
-      <c r="N72" s="108"/>
-      <c r="O72" s="108"/>
-      <c r="P72" s="108"/>
-      <c r="Q72" s="108"/>
-      <c r="R72" s="108"/>
+      <c r="A72" s="126"/>
+      <c r="B72" s="126"/>
+      <c r="C72" s="126"/>
+      <c r="D72" s="126"/>
+      <c r="E72" s="126"/>
+      <c r="F72" s="126"/>
+      <c r="G72" s="126"/>
+      <c r="H72" s="126"/>
+      <c r="I72" s="126"/>
+      <c r="J72" s="126"/>
+      <c r="K72" s="126"/>
+      <c r="L72" s="126"/>
+      <c r="M72" s="126"/>
+      <c r="N72" s="126"/>
+      <c r="O72" s="126"/>
+      <c r="P72" s="126"/>
+      <c r="Q72" s="126"/>
+      <c r="R72" s="126"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="126"/>
+      <c r="B73" s="126"/>
+      <c r="C73" s="126"/>
+      <c r="D73" s="126"/>
+      <c r="E73" s="126"/>
+      <c r="F73" s="126"/>
+      <c r="G73" s="126"/>
+      <c r="H73" s="126"/>
+      <c r="I73" s="126"/>
+      <c r="J73" s="126"/>
+      <c r="K73" s="126"/>
+      <c r="L73" s="126"/>
+      <c r="M73" s="126"/>
+      <c r="N73" s="126"/>
+      <c r="O73" s="126"/>
+      <c r="P73" s="126"/>
+      <c r="Q73" s="126"/>
+      <c r="R73" s="126"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="126"/>
+      <c r="B74" s="126"/>
+      <c r="C74" s="126"/>
+      <c r="D74" s="126"/>
+      <c r="E74" s="126"/>
+      <c r="F74" s="126"/>
+      <c r="G74" s="126"/>
+      <c r="H74" s="126"/>
+      <c r="I74" s="126"/>
+      <c r="J74" s="126"/>
+      <c r="K74" s="126"/>
+      <c r="L74" s="126"/>
+      <c r="M74" s="126"/>
+      <c r="N74" s="126"/>
+      <c r="O74" s="126"/>
+      <c r="P74" s="126"/>
+      <c r="Q74" s="126"/>
+      <c r="R74" s="126"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="126"/>
+      <c r="B75" s="126"/>
+      <c r="C75" s="126"/>
+      <c r="D75" s="126"/>
+      <c r="E75" s="126"/>
+      <c r="F75" s="126"/>
+      <c r="G75" s="126"/>
+      <c r="H75" s="126"/>
+      <c r="I75" s="126"/>
+      <c r="J75" s="126"/>
+      <c r="K75" s="126"/>
+      <c r="L75" s="126"/>
+      <c r="M75" s="126"/>
+      <c r="N75" s="126"/>
+      <c r="O75" s="126"/>
+      <c r="P75" s="126"/>
+      <c r="Q75" s="126"/>
+      <c r="R75" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="26">
@@ -5090,16 +5350,16 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="L8:N8"/>
-    <mergeCell ref="D54:N54"/>
-    <mergeCell ref="A56:B58"/>
-    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D57:N57"/>
+    <mergeCell ref="A59:B61"/>
+    <mergeCell ref="D61:F61"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="H4"/>
@@ -5116,27 +5376,29 @@
     <hyperlink r:id="rId12" ref="N30"/>
     <hyperlink r:id="rId13" ref="K31"/>
     <hyperlink r:id="rId14" ref="N31"/>
-    <hyperlink r:id="rId15" ref="K45"/>
-    <hyperlink r:id="rId16" ref="N45"/>
-    <hyperlink r:id="rId17" ref="K46"/>
-    <hyperlink r:id="rId18" ref="N46"/>
-    <hyperlink r:id="rId19" ref="K47"/>
-    <hyperlink r:id="rId20" ref="N47"/>
-    <hyperlink r:id="rId21" ref="K48"/>
-    <hyperlink r:id="rId22" ref="N48"/>
-    <hyperlink r:id="rId23" ref="K49"/>
-    <hyperlink r:id="rId24" ref="N49"/>
-    <hyperlink r:id="rId25" ref="K50"/>
-    <hyperlink r:id="rId26" ref="N50"/>
-    <hyperlink r:id="rId27" ref="K51"/>
-    <hyperlink r:id="rId28" ref="N51"/>
-    <hyperlink r:id="rId29" ref="K52"/>
-    <hyperlink r:id="rId30" ref="N52"/>
-    <hyperlink r:id="rId31" ref="K53"/>
+    <hyperlink r:id="rId15" ref="K47"/>
+    <hyperlink r:id="rId16" ref="N47"/>
+    <hyperlink r:id="rId17" ref="K48"/>
+    <hyperlink r:id="rId18" ref="N48"/>
+    <hyperlink r:id="rId19" ref="K49"/>
+    <hyperlink r:id="rId20" ref="N49"/>
+    <hyperlink r:id="rId21" ref="K50"/>
+    <hyperlink r:id="rId22" ref="N50"/>
+    <hyperlink r:id="rId23" ref="K51"/>
+    <hyperlink r:id="rId24" ref="N51"/>
+    <hyperlink r:id="rId25" ref="K52"/>
+    <hyperlink r:id="rId26" ref="N52"/>
+    <hyperlink r:id="rId27" ref="K53"/>
+    <hyperlink r:id="rId28" ref="N53"/>
+    <hyperlink r:id="rId29" ref="K54"/>
+    <hyperlink r:id="rId30" ref="N54"/>
+    <hyperlink r:id="rId31" ref="K55"/>
+    <hyperlink r:id="rId32" ref="N55"/>
+    <hyperlink r:id="rId33" ref="K56"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.25" right="0.25" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId32"/>
+  <drawing r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>